<commit_message>
Herramienta de Gestion QA
Herramienta de Gestion QA
</commit_message>
<xml_diff>
--- a/Area_de_Proceso-_PPQA/HGQA_V1.0_2015.xlsx
+++ b/Area_de_Proceso-_PPQA/HGQA_V1.0_2015.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YOSHITOMI\Google Drive\9no Ciclo\Proyecto de Desarrollo de Software I\Proyecto - Sistema de Delivery Online\Entregables\Ultima Presentacion\Area PPQA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Perochena\Documents\GitHub\UTP-GPS-ALARM\Area_de_Proceso-_PPQA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -172,7 +172,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="247">
   <si>
     <t>Analista Responsable</t>
   </si>
@@ -704,16 +704,6 @@
     <t>Jefe de Proyecto:</t>
   </si>
   <si>
-    <t>Yoshitomi Maehara
-(Jefe de Proyecto)</t>
-  </si>
-  <si>
-    <t>Adecuacion de Software de delivery Online</t>
-  </si>
-  <si>
-    <t>HM, JG, RR</t>
-  </si>
-  <si>
     <t>ICIC</t>
   </si>
   <si>
@@ -765,12 +755,6 @@
     <t>Documento de analisis</t>
   </si>
   <si>
-    <t>Fecha Efectiva: 12/07/2014</t>
-  </si>
-  <si>
-    <t>JULIO</t>
-  </si>
-  <si>
     <t>GESTION DE LA CONFIGURACION</t>
   </si>
   <si>
@@ -916,6 +900,27 @@
   </si>
   <si>
     <t>Actualizar la tabla de base de datos y actualizar el numero de productos</t>
+  </si>
+  <si>
+    <t>Fecha Efectiva: 13/10/2015</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>Julio Leonardo Paredes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UTP-GPS-ALARM </t>
+  </si>
+  <si>
+    <t>Roger Apaestegui Ortega</t>
+  </si>
+  <si>
+    <t>Analista de Calidad</t>
+  </si>
+  <si>
+    <t>OCTUBRE</t>
   </si>
 </sst>
 </file>
@@ -928,7 +933,7 @@
     <numFmt numFmtId="166" formatCode="_([$€-2]\ * #,##0.00_);_([$€-2]\ * \(#,##0.00\);_([$€-2]\ * &quot;-&quot;??_)"/>
     <numFmt numFmtId="167" formatCode="m/d/yyyy;@"/>
   </numFmts>
-  <fonts count="65">
+  <fonts count="66">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1315,6 +1320,13 @@
     <font>
       <sz val="9"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -2051,7 +2063,7 @@
     <xf numFmtId="0" fontId="33" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="244">
+  <cellXfs count="243">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="32" applyFont="1" applyProtection="1">
       <protection locked="0"/>
@@ -2579,10 +2591,6 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="8" fillId="30" borderId="10" xfId="39" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="2" fontId="8" fillId="30" borderId="10" xfId="39" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -2593,102 +2601,146 @@
     <xf numFmtId="167" fontId="62" fillId="30" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="10" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="49" fillId="0" borderId="10" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="15" fontId="8" fillId="0" borderId="10" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="40" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="10" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="44" fillId="24" borderId="0" xfId="43" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="33" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="29" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="33" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="29" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="11" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="33" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="29" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="11" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="33" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="29" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="11" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="29" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="32" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="32" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="24" borderId="0" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="33" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="29" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="24" borderId="0" xfId="36" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="33" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="29" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="11" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="33" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="29" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="11" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="33" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="29" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="11" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="29" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="32" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="32" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="11" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="29" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="24" borderId="11" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -2710,14 +2762,6 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="11" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="29" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="44" fillId="24" borderId="34" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -2730,6 +2774,57 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="56" fillId="25" borderId="10" xfId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="25" borderId="13" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="25" borderId="37" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="24" borderId="11" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="24" borderId="33" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="24" borderId="29" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="25" borderId="10" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="25" borderId="10" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="49" fillId="24" borderId="13" xfId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="49" fillId="24" borderId="37" xfId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="25" borderId="13" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="25" borderId="37" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="25" borderId="11" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="44" fillId="24" borderId="0" xfId="32" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -2738,18 +2833,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="24" borderId="11" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="24" borderId="33" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="24" borderId="29" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="45" fillId="25" borderId="11" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -2758,45 +2841,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="56" fillId="25" borderId="10" xfId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="25" borderId="13" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="25" borderId="37" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="25" borderId="10" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="25" borderId="10" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="49" fillId="24" borderId="13" xfId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="49" fillId="24" borderId="37" xfId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="25" borderId="13" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="25" borderId="37" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="25" borderId="11" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="58" fillId="0" borderId="10" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2809,44 +2853,8 @@
     <xf numFmtId="0" fontId="58" fillId="0" borderId="40" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="11" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="10" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="49" fillId="0" borderId="10" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="15" fontId="8" fillId="0" borderId="10" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="40" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="64" fillId="0" borderId="10" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="53">
@@ -3051,7 +3059,7 @@
                     <a:cs typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="es-MX"/>
+                <a:endParaRPr lang="es-PE"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
@@ -3062,7 +3070,9 @@
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="1"/>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -3150,7 +3160,7 @@
               <a:cs typeface="Arial"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-MX"/>
+          <a:endParaRPr lang="es-PE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3183,7 +3193,7 @@
           <a:cs typeface="Arial"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="es-MX"/>
+      <a:endParaRPr lang="es-PE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3379,7 +3389,9 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -3398,7 +3410,9 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -3417,7 +3431,9 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:numFmt formatCode="0%" sourceLinked="0"/>
@@ -3441,7 +3457,7 @@
                     <a:cs typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="es-MX"/>
+                <a:endParaRPr lang="es-PE"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="1"/>
@@ -3452,7 +3468,9 @@
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -3558,7 +3576,7 @@
               <a:cs typeface="Arial"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-MX"/>
+          <a:endParaRPr lang="es-PE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3591,7 +3609,7 @@
           <a:cs typeface="Arial"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="es-MX"/>
+      <a:endParaRPr lang="es-PE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3773,7 +3791,7 @@
                     <a:cs typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="es-MX"/>
+                <a:endParaRPr lang="es-PE"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="ctr"/>
@@ -3786,6 +3804,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -3829,11 +3848,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="790444960"/>
-        <c:axId val="790436256"/>
+        <c:axId val="175517376"/>
+        <c:axId val="175517936"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="790444960"/>
+        <c:axId val="175517376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3865,10 +3884,10 @@
                 <a:cs typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-MX"/>
+            <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="790436256"/>
+        <c:crossAx val="175517936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3878,7 +3897,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="790436256"/>
+        <c:axId val="175517936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3920,10 +3939,10 @@
                 <a:cs typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-MX"/>
+            <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="790444960"/>
+        <c:crossAx val="175517376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3977,7 +3996,7 @@
               <a:cs typeface="Arial"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-MX"/>
+          <a:endParaRPr lang="es-PE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4010,7 +4029,7 @@
           <a:cs typeface="Arial"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="es-MX"/>
+      <a:endParaRPr lang="es-PE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4187,7 +4206,7 @@
                     <a:cs typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="es-MX"/>
+                <a:endParaRPr lang="es-PE"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
@@ -4263,7 +4282,7 @@
                     <a:cs typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="es-MX"/>
+                <a:endParaRPr lang="es-PE"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
@@ -4339,7 +4358,7 @@
                     <a:cs typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="es-MX"/>
+                <a:endParaRPr lang="es-PE"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
@@ -4378,12 +4397,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="790437888"/>
-        <c:axId val="790444416"/>
+        <c:axId val="175521296"/>
+        <c:axId val="175821248"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="790437888"/>
+        <c:axId val="175521296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4454,10 +4473,10 @@
                 <a:cs typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-MX"/>
+            <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="790444416"/>
+        <c:crossAx val="175821248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4467,7 +4486,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="790444416"/>
+        <c:axId val="175821248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4548,10 +4567,10 @@
                 <a:cs typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-MX"/>
+            <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="790437888"/>
+        <c:crossAx val="175521296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4600,7 +4619,7 @@
               <a:cs typeface="Arial"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-MX"/>
+          <a:endParaRPr lang="es-PE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4633,7 +4652,7 @@
           <a:cs typeface="Arial"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="es-MX"/>
+      <a:endParaRPr lang="es-PE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4645,58 +4664,6 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="1 Imagen" descr="C:\Users\Yoshitomi\Google Drive\9no Ciclo\Proyecto de Desarrollo de Software I\Proyecto - Sistema de Servicios de Restaurantes\logo.jpg"/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="314325" y="0"/>
-          <a:ext cx="1171575" cy="771525"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4744,57 +4711,10 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>771525</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="2 Imagen" descr="C:\Users\Yoshitomi\Google Drive\9no Ciclo\Proyecto de Desarrollo de Software I\Proyecto - Sistema de Servicios de Restaurantes\logo.jpg"/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="9525" y="0"/>
-          <a:ext cx="1171575" cy="771525"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4922,53 +4842,6 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>866775</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>390525</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="5 Imagen" descr="C:\Users\Yoshitomi\Google Drive\9no Ciclo\Proyecto de Desarrollo de Software I\Proyecto - Sistema de Servicios de Restaurantes\logo.jpg"/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="1171575" cy="771525"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -5334,7 +5207,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -5363,15 +5236,15 @@
     </row>
     <row r="2" spans="1:9" ht="15.75">
       <c r="A2" s="67"/>
-      <c r="B2" s="170" t="s">
+      <c r="B2" s="180" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="170"/>
-      <c r="D2" s="170"/>
-      <c r="E2" s="170"/>
-      <c r="F2" s="170"/>
-      <c r="G2" s="170"/>
-      <c r="H2" s="170"/>
+      <c r="C2" s="180"/>
+      <c r="D2" s="180"/>
+      <c r="E2" s="180"/>
+      <c r="F2" s="180"/>
+      <c r="G2" s="180"/>
+      <c r="H2" s="180"/>
       <c r="I2" s="67"/>
     </row>
     <row r="3" spans="1:9" ht="13.5" thickBot="1">
@@ -5410,22 +5283,22 @@
       </c>
       <c r="I4" s="67"/>
     </row>
-    <row r="5" spans="1:9" ht="36">
+    <row r="5" spans="1:9" ht="24">
       <c r="A5" s="67"/>
       <c r="B5" s="72">
         <v>1</v>
       </c>
-      <c r="C5" s="73">
-        <v>0.1</v>
+      <c r="C5" s="73" t="s">
+        <v>241</v>
       </c>
       <c r="D5" s="74">
-        <v>41832</v>
+        <v>42290</v>
       </c>
       <c r="E5" s="75" t="s">
-        <v>174</v>
+        <v>242</v>
       </c>
       <c r="F5" s="75" t="s">
-        <v>175</v>
+        <v>243</v>
       </c>
       <c r="G5" s="76" t="s">
         <v>69</v>
@@ -5504,8 +5377,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:M87"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27:E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -5522,22 +5395,22 @@
     <row r="2" spans="1:8" s="62" customFormat="1" ht="48.75" customHeight="1">
       <c r="A2" s="39"/>
       <c r="B2" s="63"/>
-      <c r="C2" s="191" t="s">
+      <c r="C2" s="242" t="s">
         <v>164</v>
       </c>
-      <c r="D2" s="192"/>
-      <c r="E2" s="193"/>
+      <c r="D2" s="193"/>
+      <c r="E2" s="194"/>
     </row>
     <row r="3" spans="1:8" s="62" customFormat="1">
       <c r="A3" s="39"/>
       <c r="B3" s="64" t="s">
         <v>94</v>
       </c>
-      <c r="C3" s="199" t="s">
-        <v>194</v>
-      </c>
-      <c r="D3" s="200"/>
-      <c r="E3" s="201"/>
+      <c r="C3" s="200" t="s">
+        <v>240</v>
+      </c>
+      <c r="D3" s="201"/>
+      <c r="E3" s="202"/>
     </row>
     <row r="4" spans="1:8" s="62" customFormat="1" ht="21.75" customHeight="1">
       <c r="A4" s="39"/>
@@ -5549,12 +5422,12 @@
     </row>
     <row r="5" spans="1:8" ht="24.75" customHeight="1">
       <c r="A5" s="39"/>
-      <c r="B5" s="194" t="s">
+      <c r="B5" s="195" t="s">
         <v>70</v>
       </c>
-      <c r="C5" s="195"/>
-      <c r="D5" s="195"/>
-      <c r="E5" s="196"/>
+      <c r="C5" s="196"/>
+      <c r="D5" s="196"/>
+      <c r="E5" s="197"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="39"/>
@@ -5577,10 +5450,10 @@
         <v>5</v>
       </c>
       <c r="C8" s="92"/>
-      <c r="D8" s="197" t="s">
+      <c r="D8" s="198" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="198"/>
+      <c r="E8" s="199"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="39"/>
@@ -5666,62 +5539,62 @@
       <c r="A18" s="37"/>
     </row>
     <row r="19" spans="1:8" s="58" customFormat="1" ht="16.5" customHeight="1">
-      <c r="B19" s="185" t="s">
+      <c r="B19" s="187" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="186"/>
-      <c r="D19" s="186"/>
-      <c r="E19" s="187"/>
+      <c r="C19" s="188"/>
+      <c r="D19" s="188"/>
+      <c r="E19" s="189"/>
     </row>
     <row r="20" spans="1:8" s="58" customFormat="1" ht="13.5" customHeight="1">
       <c r="B20" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="C20" s="188" t="s">
+      <c r="C20" s="190" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="189"/>
-      <c r="E20" s="190"/>
+      <c r="D20" s="191"/>
+      <c r="E20" s="192"/>
     </row>
     <row r="21" spans="1:8" s="58" customFormat="1" ht="12.75" customHeight="1">
       <c r="B21" s="59" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="176" t="s">
+      <c r="C21" s="203" t="s">
         <v>49</v>
       </c>
-      <c r="D21" s="177"/>
-      <c r="E21" s="178"/>
+      <c r="D21" s="204"/>
+      <c r="E21" s="205"/>
     </row>
     <row r="22" spans="1:8" s="58" customFormat="1" ht="12.75" customHeight="1">
       <c r="B22" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="176" t="s">
+      <c r="C22" s="203" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="177"/>
-      <c r="E22" s="178"/>
+      <c r="D22" s="204"/>
+      <c r="E22" s="205"/>
     </row>
     <row r="23" spans="1:8" s="58" customFormat="1" ht="12.75" customHeight="1">
       <c r="B23" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="176" t="s">
+      <c r="C23" s="203" t="s">
         <v>101</v>
       </c>
-      <c r="D23" s="177"/>
-      <c r="E23" s="178"/>
+      <c r="D23" s="204"/>
+      <c r="E23" s="205"/>
     </row>
     <row r="24" spans="1:8" s="58" customFormat="1" ht="13.5" customHeight="1">
       <c r="B24" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="176" t="s">
+      <c r="C24" s="203" t="s">
         <v>8</v>
       </c>
-      <c r="D24" s="177"/>
-      <c r="E24" s="178"/>
+      <c r="D24" s="204"/>
+      <c r="E24" s="205"/>
     </row>
     <row r="25" spans="1:8" s="58" customFormat="1" ht="13.5" customHeight="1">
       <c r="B25" s="60"/>
@@ -5734,31 +5607,31 @@
       <c r="B26" s="51"/>
     </row>
     <row r="27" spans="1:8" s="58" customFormat="1" ht="16.5" customHeight="1">
-      <c r="B27" s="185" t="s">
+      <c r="B27" s="187" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="186"/>
-      <c r="D27" s="186"/>
-      <c r="E27" s="187"/>
+      <c r="C27" s="188"/>
+      <c r="D27" s="188"/>
+      <c r="E27" s="189"/>
     </row>
     <row r="28" spans="1:8" s="58" customFormat="1" ht="13.5" customHeight="1">
       <c r="B28" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="C28" s="188" t="s">
+      <c r="C28" s="190" t="s">
         <v>6</v>
       </c>
-      <c r="D28" s="189"/>
-      <c r="E28" s="190"/>
+      <c r="D28" s="191"/>
+      <c r="E28" s="192"/>
     </row>
     <row r="29" spans="1:8" ht="12.75" customHeight="1">
       <c r="A29" s="37"/>
-      <c r="B29" s="182" t="s">
+      <c r="B29" s="206" t="s">
         <v>50</v>
       </c>
-      <c r="C29" s="183"/>
-      <c r="D29" s="183"/>
-      <c r="E29" s="184"/>
+      <c r="C29" s="207"/>
+      <c r="D29" s="207"/>
+      <c r="E29" s="208"/>
       <c r="F29" s="58"/>
       <c r="G29" s="58"/>
     </row>
@@ -5767,11 +5640,11 @@
       <c r="B30" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="C30" s="172" t="s">
+      <c r="C30" s="181" t="s">
         <v>114</v>
       </c>
-      <c r="D30" s="173"/>
-      <c r="E30" s="174"/>
+      <c r="D30" s="182"/>
+      <c r="E30" s="183"/>
       <c r="F30" s="58"/>
       <c r="G30" s="58"/>
     </row>
@@ -5780,11 +5653,11 @@
       <c r="B31" s="46" t="s">
         <v>115</v>
       </c>
-      <c r="C31" s="172" t="s">
+      <c r="C31" s="181" t="s">
         <v>116</v>
       </c>
-      <c r="D31" s="173"/>
-      <c r="E31" s="174"/>
+      <c r="D31" s="182"/>
+      <c r="E31" s="183"/>
       <c r="F31" s="58"/>
       <c r="G31" s="58"/>
     </row>
@@ -5793,11 +5666,11 @@
       <c r="B32" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="172" t="s">
+      <c r="C32" s="181" t="s">
         <v>53</v>
       </c>
-      <c r="D32" s="173"/>
-      <c r="E32" s="174"/>
+      <c r="D32" s="182"/>
+      <c r="E32" s="183"/>
       <c r="F32" s="58"/>
       <c r="G32" s="58"/>
     </row>
@@ -5806,11 +5679,11 @@
       <c r="B33" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="C33" s="172" t="s">
+      <c r="C33" s="181" t="s">
         <v>72</v>
       </c>
-      <c r="D33" s="173"/>
-      <c r="E33" s="174"/>
+      <c r="D33" s="182"/>
+      <c r="E33" s="183"/>
       <c r="F33" s="58"/>
       <c r="G33" s="58"/>
     </row>
@@ -5819,174 +5692,174 @@
       <c r="B34" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C34" s="172" t="s">
+      <c r="C34" s="181" t="s">
         <v>73</v>
       </c>
-      <c r="D34" s="173"/>
-      <c r="E34" s="174"/>
+      <c r="D34" s="182"/>
+      <c r="E34" s="183"/>
     </row>
     <row r="35" spans="1:7" ht="16.5" customHeight="1">
       <c r="A35" s="37"/>
       <c r="B35" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="C35" s="172" t="s">
+      <c r="C35" s="181" t="s">
         <v>74</v>
       </c>
-      <c r="D35" s="173"/>
-      <c r="E35" s="174"/>
+      <c r="D35" s="182"/>
+      <c r="E35" s="183"/>
     </row>
     <row r="36" spans="1:7" ht="16.5" customHeight="1">
       <c r="A36" s="37"/>
-      <c r="B36" s="182" t="s">
+      <c r="B36" s="206" t="s">
         <v>51</v>
       </c>
-      <c r="C36" s="183"/>
-      <c r="D36" s="183"/>
-      <c r="E36" s="184"/>
+      <c r="C36" s="207"/>
+      <c r="D36" s="207"/>
+      <c r="E36" s="208"/>
     </row>
     <row r="37" spans="1:7" ht="16.5" customHeight="1">
       <c r="A37" s="37"/>
       <c r="B37" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="C37" s="172" t="s">
+      <c r="C37" s="181" t="s">
         <v>75</v>
       </c>
-      <c r="D37" s="173"/>
-      <c r="E37" s="174"/>
+      <c r="D37" s="182"/>
+      <c r="E37" s="183"/>
     </row>
     <row r="38" spans="1:7" ht="16.5" customHeight="1">
       <c r="A38" s="37"/>
       <c r="B38" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="C38" s="172" t="s">
+      <c r="C38" s="181" t="s">
         <v>86</v>
       </c>
-      <c r="D38" s="173"/>
-      <c r="E38" s="174"/>
+      <c r="D38" s="182"/>
+      <c r="E38" s="183"/>
     </row>
     <row r="39" spans="1:7" ht="17.25" customHeight="1">
       <c r="A39" s="37"/>
       <c r="B39" s="46" t="s">
         <v>102</v>
       </c>
-      <c r="C39" s="172" t="s">
+      <c r="C39" s="181" t="s">
         <v>103</v>
       </c>
-      <c r="D39" s="173"/>
-      <c r="E39" s="174"/>
+      <c r="D39" s="182"/>
+      <c r="E39" s="183"/>
     </row>
     <row r="40" spans="1:7" ht="16.5" customHeight="1">
       <c r="A40" s="37"/>
       <c r="B40" s="46" t="s">
         <v>148</v>
       </c>
-      <c r="C40" s="172" t="s">
+      <c r="C40" s="181" t="s">
         <v>149</v>
       </c>
-      <c r="D40" s="173"/>
-      <c r="E40" s="174"/>
+      <c r="D40" s="182"/>
+      <c r="E40" s="183"/>
     </row>
     <row r="41" spans="1:7" ht="16.5" customHeight="1">
       <c r="A41" s="37"/>
       <c r="B41" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="C41" s="172" t="s">
+      <c r="C41" s="181" t="s">
         <v>105</v>
       </c>
-      <c r="D41" s="173"/>
-      <c r="E41" s="174"/>
+      <c r="D41" s="182"/>
+      <c r="E41" s="183"/>
     </row>
     <row r="42" spans="1:7" ht="16.5" customHeight="1">
       <c r="A42" s="37"/>
       <c r="B42" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="C42" s="172" t="s">
+      <c r="C42" s="181" t="s">
         <v>104</v>
       </c>
-      <c r="D42" s="173"/>
-      <c r="E42" s="174"/>
+      <c r="D42" s="182"/>
+      <c r="E42" s="183"/>
     </row>
     <row r="43" spans="1:7" ht="16.5" customHeight="1">
       <c r="A43" s="37"/>
       <c r="B43" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="C43" s="172" t="s">
+      <c r="C43" s="181" t="s">
         <v>78</v>
       </c>
-      <c r="D43" s="173"/>
-      <c r="E43" s="174"/>
+      <c r="D43" s="182"/>
+      <c r="E43" s="183"/>
     </row>
     <row r="44" spans="1:7" ht="16.5" customHeight="1">
       <c r="A44" s="37"/>
       <c r="B44" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="C44" s="172" t="s">
+      <c r="C44" s="181" t="s">
         <v>79</v>
       </c>
-      <c r="D44" s="173"/>
-      <c r="E44" s="174"/>
+      <c r="D44" s="182"/>
+      <c r="E44" s="183"/>
     </row>
     <row r="45" spans="1:7" ht="16.5" customHeight="1">
       <c r="A45" s="37"/>
       <c r="B45" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="C45" s="172" t="s">
+      <c r="C45" s="181" t="s">
         <v>76</v>
       </c>
-      <c r="D45" s="173"/>
-      <c r="E45" s="174"/>
+      <c r="D45" s="182"/>
+      <c r="E45" s="183"/>
     </row>
     <row r="46" spans="1:7" ht="16.5" customHeight="1">
       <c r="A46" s="37"/>
       <c r="B46" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="C46" s="172" t="s">
+      <c r="C46" s="181" t="s">
         <v>81</v>
       </c>
-      <c r="D46" s="173"/>
-      <c r="E46" s="174"/>
+      <c r="D46" s="182"/>
+      <c r="E46" s="183"/>
     </row>
     <row r="47" spans="1:7" ht="16.5" customHeight="1">
       <c r="A47" s="37"/>
       <c r="B47" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="C47" s="172" t="s">
+      <c r="C47" s="181" t="s">
         <v>82</v>
       </c>
-      <c r="D47" s="173"/>
-      <c r="E47" s="174"/>
+      <c r="D47" s="182"/>
+      <c r="E47" s="183"/>
     </row>
     <row r="48" spans="1:7" ht="16.5" customHeight="1">
       <c r="A48" s="37"/>
       <c r="B48" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="C48" s="172" t="s">
+      <c r="C48" s="181" t="s">
         <v>80</v>
       </c>
-      <c r="D48" s="173"/>
-      <c r="E48" s="174"/>
+      <c r="D48" s="182"/>
+      <c r="E48" s="183"/>
     </row>
     <row r="49" spans="1:13" ht="16.5" customHeight="1">
       <c r="A49" s="37"/>
       <c r="B49" s="46" t="s">
         <v>150</v>
       </c>
-      <c r="C49" s="172" t="s">
+      <c r="C49" s="181" t="s">
         <v>77</v>
       </c>
-      <c r="D49" s="173"/>
-      <c r="E49" s="174"/>
+      <c r="D49" s="182"/>
+      <c r="E49" s="183"/>
     </row>
     <row r="50" spans="1:13" ht="16.5" customHeight="1">
       <c r="A50" s="58"/>
@@ -6019,23 +5892,23 @@
       <c r="M51" s="38"/>
     </row>
     <row r="52" spans="1:13" s="58" customFormat="1" ht="16.5" customHeight="1">
-      <c r="B52" s="185" t="s">
+      <c r="B52" s="187" t="s">
         <v>54</v>
       </c>
-      <c r="C52" s="186"/>
-      <c r="D52" s="186"/>
-      <c r="E52" s="187"/>
+      <c r="C52" s="188"/>
+      <c r="D52" s="188"/>
+      <c r="E52" s="189"/>
     </row>
     <row r="53" spans="1:13" ht="16.5" customHeight="1">
       <c r="A53" s="58"/>
       <c r="B53" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="C53" s="188" t="s">
+      <c r="C53" s="190" t="s">
         <v>6</v>
       </c>
-      <c r="D53" s="189"/>
-      <c r="E53" s="190"/>
+      <c r="D53" s="191"/>
+      <c r="E53" s="192"/>
       <c r="F53" s="58"/>
       <c r="G53" s="58"/>
       <c r="H53" s="58"/>
@@ -6050,132 +5923,132 @@
       <c r="B54" s="46" t="s">
         <v>151</v>
       </c>
-      <c r="C54" s="172" t="s">
+      <c r="C54" s="181" t="s">
         <v>75</v>
       </c>
-      <c r="D54" s="173"/>
-      <c r="E54" s="174"/>
+      <c r="D54" s="182"/>
+      <c r="E54" s="183"/>
     </row>
     <row r="55" spans="1:13" ht="16.5" customHeight="1">
       <c r="A55" s="37"/>
       <c r="B55" s="46" t="s">
         <v>124</v>
       </c>
-      <c r="C55" s="172" t="s">
+      <c r="C55" s="181" t="s">
         <v>87</v>
       </c>
-      <c r="D55" s="173"/>
-      <c r="E55" s="174"/>
+      <c r="D55" s="182"/>
+      <c r="E55" s="183"/>
     </row>
     <row r="56" spans="1:13" ht="16.5" customHeight="1">
       <c r="A56" s="37"/>
       <c r="B56" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="C56" s="172" t="s">
+      <c r="C56" s="181" t="s">
         <v>88</v>
       </c>
-      <c r="D56" s="173"/>
-      <c r="E56" s="174"/>
+      <c r="D56" s="182"/>
+      <c r="E56" s="183"/>
     </row>
     <row r="57" spans="1:13" ht="16.5" customHeight="1">
       <c r="A57" s="37"/>
       <c r="B57" s="46" t="s">
         <v>112</v>
       </c>
-      <c r="C57" s="172" t="s">
+      <c r="C57" s="181" t="s">
         <v>106</v>
       </c>
-      <c r="D57" s="179"/>
-      <c r="E57" s="180"/>
+      <c r="D57" s="185"/>
+      <c r="E57" s="186"/>
     </row>
     <row r="58" spans="1:13" ht="16.5" customHeight="1">
       <c r="A58" s="37"/>
       <c r="B58" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="C58" s="172" t="s">
+      <c r="C58" s="181" t="s">
         <v>92</v>
       </c>
-      <c r="D58" s="179"/>
-      <c r="E58" s="180"/>
+      <c r="D58" s="185"/>
+      <c r="E58" s="186"/>
     </row>
     <row r="59" spans="1:13" ht="16.5" customHeight="1">
       <c r="A59" s="37"/>
       <c r="B59" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="C59" s="172" t="s">
+      <c r="C59" s="181" t="s">
         <v>83</v>
       </c>
-      <c r="D59" s="179"/>
-      <c r="E59" s="180"/>
+      <c r="D59" s="185"/>
+      <c r="E59" s="186"/>
     </row>
     <row r="60" spans="1:13" ht="54" customHeight="1">
       <c r="A60" s="37"/>
       <c r="B60" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="C60" s="172" t="s">
+      <c r="C60" s="181" t="s">
         <v>107</v>
       </c>
-      <c r="D60" s="179"/>
-      <c r="E60" s="180"/>
+      <c r="D60" s="185"/>
+      <c r="E60" s="186"/>
     </row>
     <row r="61" spans="1:13" ht="16.5" customHeight="1">
       <c r="A61" s="37"/>
       <c r="B61" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="C61" s="181" t="s">
+      <c r="C61" s="184" t="s">
         <v>91</v>
       </c>
-      <c r="D61" s="179"/>
-      <c r="E61" s="180"/>
+      <c r="D61" s="185"/>
+      <c r="E61" s="186"/>
     </row>
     <row r="62" spans="1:13" ht="30" customHeight="1">
       <c r="A62" s="37"/>
       <c r="B62" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="C62" s="172" t="s">
+      <c r="C62" s="181" t="s">
         <v>56</v>
       </c>
-      <c r="D62" s="179"/>
-      <c r="E62" s="180"/>
+      <c r="D62" s="185"/>
+      <c r="E62" s="186"/>
     </row>
     <row r="63" spans="1:13" ht="16.5" customHeight="1">
       <c r="A63" s="37"/>
       <c r="B63" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="C63" s="181" t="s">
+      <c r="C63" s="184" t="s">
         <v>61</v>
       </c>
-      <c r="D63" s="179"/>
-      <c r="E63" s="180"/>
+      <c r="D63" s="185"/>
+      <c r="E63" s="186"/>
     </row>
     <row r="64" spans="1:13" ht="16.5" customHeight="1">
       <c r="A64" s="37"/>
       <c r="B64" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="C64" s="181" t="s">
+      <c r="C64" s="184" t="s">
         <v>84</v>
       </c>
-      <c r="D64" s="179"/>
-      <c r="E64" s="180"/>
+      <c r="D64" s="185"/>
+      <c r="E64" s="186"/>
     </row>
     <row r="65" spans="1:8" ht="16.5" customHeight="1">
       <c r="A65" s="37"/>
       <c r="B65" s="46" t="s">
         <v>99</v>
       </c>
-      <c r="C65" s="172" t="s">
+      <c r="C65" s="181" t="s">
         <v>77</v>
       </c>
-      <c r="D65" s="173"/>
-      <c r="E65" s="174"/>
+      <c r="D65" s="182"/>
+      <c r="E65" s="183"/>
     </row>
     <row r="66" spans="1:8" ht="16.5" customHeight="1">
       <c r="A66" s="37"/>
@@ -6186,200 +6059,200 @@
     </row>
     <row r="67" spans="1:8" ht="16.5" customHeight="1">
       <c r="A67" s="37"/>
-      <c r="B67" s="175"/>
-      <c r="C67" s="175"/>
-      <c r="D67" s="175"/>
-      <c r="E67" s="175"/>
+      <c r="B67" s="210"/>
+      <c r="C67" s="210"/>
+      <c r="D67" s="210"/>
+      <c r="E67" s="210"/>
       <c r="F67" s="57"/>
       <c r="G67" s="57"/>
       <c r="H67" s="57"/>
     </row>
     <row r="68" spans="1:8" ht="16.5" customHeight="1">
       <c r="A68" s="37"/>
-      <c r="B68" s="171"/>
-      <c r="C68" s="171"/>
-      <c r="D68" s="171"/>
-      <c r="E68" s="171"/>
+      <c r="B68" s="209"/>
+      <c r="C68" s="209"/>
+      <c r="D68" s="209"/>
+      <c r="E68" s="209"/>
       <c r="F68" s="57"/>
       <c r="G68" s="57"/>
       <c r="H68" s="57"/>
     </row>
     <row r="69" spans="1:8" ht="16.5" customHeight="1">
       <c r="A69" s="37"/>
-      <c r="B69" s="171"/>
-      <c r="C69" s="171"/>
-      <c r="D69" s="171"/>
-      <c r="E69" s="171"/>
+      <c r="B69" s="209"/>
+      <c r="C69" s="209"/>
+      <c r="D69" s="209"/>
+      <c r="E69" s="209"/>
       <c r="F69" s="57"/>
       <c r="G69" s="57"/>
       <c r="H69" s="57"/>
     </row>
     <row r="70" spans="1:8" ht="16.5" customHeight="1">
       <c r="A70" s="37"/>
-      <c r="B70" s="171"/>
-      <c r="C70" s="171"/>
-      <c r="D70" s="171"/>
-      <c r="E70" s="171"/>
+      <c r="B70" s="209"/>
+      <c r="C70" s="209"/>
+      <c r="D70" s="209"/>
+      <c r="E70" s="209"/>
       <c r="F70" s="57"/>
       <c r="G70" s="57"/>
       <c r="H70" s="57"/>
     </row>
     <row r="71" spans="1:8" ht="16.5" customHeight="1">
       <c r="A71" s="37"/>
-      <c r="B71" s="171"/>
-      <c r="C71" s="171"/>
-      <c r="D71" s="171"/>
-      <c r="E71" s="171"/>
+      <c r="B71" s="209"/>
+      <c r="C71" s="209"/>
+      <c r="D71" s="209"/>
+      <c r="E71" s="209"/>
       <c r="F71" s="57"/>
       <c r="G71" s="57"/>
       <c r="H71" s="57"/>
     </row>
     <row r="72" spans="1:8" ht="16.5" customHeight="1">
       <c r="A72" s="37"/>
-      <c r="B72" s="171"/>
-      <c r="C72" s="171"/>
-      <c r="D72" s="171"/>
-      <c r="E72" s="171"/>
+      <c r="B72" s="209"/>
+      <c r="C72" s="209"/>
+      <c r="D72" s="209"/>
+      <c r="E72" s="209"/>
       <c r="F72" s="57"/>
       <c r="G72" s="57"/>
       <c r="H72" s="57"/>
     </row>
     <row r="73" spans="1:8" ht="16.5" customHeight="1">
       <c r="A73" s="42"/>
-      <c r="B73" s="171"/>
-      <c r="C73" s="171"/>
-      <c r="D73" s="171"/>
-      <c r="E73" s="171"/>
+      <c r="B73" s="209"/>
+      <c r="C73" s="209"/>
+      <c r="D73" s="209"/>
+      <c r="E73" s="209"/>
       <c r="F73" s="57"/>
       <c r="G73" s="57"/>
       <c r="H73" s="57"/>
     </row>
     <row r="74" spans="1:8" ht="16.5" customHeight="1">
       <c r="A74" s="37"/>
-      <c r="B74" s="171"/>
-      <c r="C74" s="171"/>
-      <c r="D74" s="171"/>
-      <c r="E74" s="171"/>
+      <c r="B74" s="209"/>
+      <c r="C74" s="209"/>
+      <c r="D74" s="209"/>
+      <c r="E74" s="209"/>
       <c r="F74" s="57"/>
       <c r="G74" s="57"/>
       <c r="H74" s="57"/>
     </row>
     <row r="75" spans="1:8" ht="16.5" customHeight="1">
       <c r="A75" s="37"/>
-      <c r="B75" s="171"/>
-      <c r="C75" s="171"/>
-      <c r="D75" s="171"/>
-      <c r="E75" s="171"/>
+      <c r="B75" s="209"/>
+      <c r="C75" s="209"/>
+      <c r="D75" s="209"/>
+      <c r="E75" s="209"/>
       <c r="F75" s="57"/>
       <c r="G75" s="57"/>
       <c r="H75" s="57"/>
     </row>
     <row r="76" spans="1:8" ht="16.5" customHeight="1">
       <c r="A76" s="37"/>
-      <c r="B76" s="171"/>
-      <c r="C76" s="171"/>
-      <c r="D76" s="171"/>
-      <c r="E76" s="171"/>
+      <c r="B76" s="209"/>
+      <c r="C76" s="209"/>
+      <c r="D76" s="209"/>
+      <c r="E76" s="209"/>
       <c r="F76" s="57"/>
       <c r="G76" s="57"/>
       <c r="H76" s="57"/>
     </row>
     <row r="77" spans="1:8" ht="16.5" customHeight="1">
       <c r="A77" s="37"/>
-      <c r="B77" s="171"/>
-      <c r="C77" s="171"/>
-      <c r="D77" s="171"/>
-      <c r="E77" s="171"/>
+      <c r="B77" s="209"/>
+      <c r="C77" s="209"/>
+      <c r="D77" s="209"/>
+      <c r="E77" s="209"/>
       <c r="F77" s="57"/>
       <c r="G77" s="57"/>
       <c r="H77" s="57"/>
     </row>
     <row r="78" spans="1:8" ht="16.5" customHeight="1">
       <c r="A78" s="37"/>
-      <c r="B78" s="171"/>
-      <c r="C78" s="171"/>
-      <c r="D78" s="171"/>
-      <c r="E78" s="171"/>
+      <c r="B78" s="209"/>
+      <c r="C78" s="209"/>
+      <c r="D78" s="209"/>
+      <c r="E78" s="209"/>
       <c r="F78" s="57"/>
       <c r="G78" s="57"/>
       <c r="H78" s="57"/>
     </row>
     <row r="79" spans="1:8" ht="16.5" customHeight="1">
       <c r="A79" s="42"/>
-      <c r="B79" s="171"/>
-      <c r="C79" s="171"/>
-      <c r="D79" s="171"/>
-      <c r="E79" s="171"/>
+      <c r="B79" s="209"/>
+      <c r="C79" s="209"/>
+      <c r="D79" s="209"/>
+      <c r="E79" s="209"/>
       <c r="F79" s="57"/>
       <c r="G79" s="57"/>
       <c r="H79" s="57"/>
     </row>
     <row r="80" spans="1:8" ht="16.5" customHeight="1">
       <c r="A80" s="42"/>
-      <c r="B80" s="171"/>
-      <c r="C80" s="171"/>
-      <c r="D80" s="171"/>
-      <c r="E80" s="171"/>
+      <c r="B80" s="209"/>
+      <c r="C80" s="209"/>
+      <c r="D80" s="209"/>
+      <c r="E80" s="209"/>
       <c r="F80" s="57"/>
       <c r="G80" s="57"/>
       <c r="H80" s="57"/>
     </row>
     <row r="81" spans="1:8" ht="16.5" customHeight="1">
       <c r="A81" s="42"/>
-      <c r="B81" s="171"/>
-      <c r="C81" s="171"/>
-      <c r="D81" s="171"/>
-      <c r="E81" s="171"/>
+      <c r="B81" s="209"/>
+      <c r="C81" s="209"/>
+      <c r="D81" s="209"/>
+      <c r="E81" s="209"/>
       <c r="F81" s="57"/>
       <c r="G81" s="57"/>
       <c r="H81" s="57"/>
     </row>
     <row r="82" spans="1:8" ht="16.5" customHeight="1">
       <c r="A82" s="42"/>
-      <c r="B82" s="171"/>
-      <c r="C82" s="171"/>
-      <c r="D82" s="171"/>
-      <c r="E82" s="171"/>
+      <c r="B82" s="209"/>
+      <c r="C82" s="209"/>
+      <c r="D82" s="209"/>
+      <c r="E82" s="209"/>
       <c r="F82" s="57"/>
       <c r="G82" s="57"/>
       <c r="H82" s="57"/>
     </row>
     <row r="83" spans="1:8" ht="16.5" customHeight="1">
       <c r="A83" s="42"/>
-      <c r="B83" s="171"/>
-      <c r="C83" s="171"/>
-      <c r="D83" s="171"/>
-      <c r="E83" s="171"/>
+      <c r="B83" s="209"/>
+      <c r="C83" s="209"/>
+      <c r="D83" s="209"/>
+      <c r="E83" s="209"/>
       <c r="F83" s="57"/>
       <c r="G83" s="57"/>
       <c r="H83" s="57"/>
     </row>
     <row r="84" spans="1:8" ht="16.5" customHeight="1">
       <c r="A84" s="42"/>
-      <c r="B84" s="171"/>
-      <c r="C84" s="171"/>
-      <c r="D84" s="171"/>
-      <c r="E84" s="171"/>
+      <c r="B84" s="209"/>
+      <c r="C84" s="209"/>
+      <c r="D84" s="209"/>
+      <c r="E84" s="209"/>
       <c r="F84" s="57"/>
       <c r="G84" s="57"/>
       <c r="H84" s="57"/>
     </row>
     <row r="85" spans="1:8" ht="16.5" customHeight="1">
       <c r="A85" s="42"/>
-      <c r="B85" s="171"/>
-      <c r="C85" s="171"/>
-      <c r="D85" s="171"/>
-      <c r="E85" s="171"/>
+      <c r="B85" s="209"/>
+      <c r="C85" s="209"/>
+      <c r="D85" s="209"/>
+      <c r="E85" s="209"/>
       <c r="F85" s="57"/>
       <c r="G85" s="57"/>
       <c r="H85" s="57"/>
     </row>
     <row r="86" spans="1:8" ht="16.5" customHeight="1">
       <c r="A86" s="42"/>
-      <c r="B86" s="171"/>
-      <c r="C86" s="171"/>
-      <c r="D86" s="171"/>
-      <c r="E86" s="171"/>
+      <c r="B86" s="209"/>
+      <c r="C86" s="209"/>
+      <c r="D86" s="209"/>
+      <c r="E86" s="209"/>
       <c r="F86" s="57"/>
       <c r="G86" s="57"/>
       <c r="H86" s="57"/>
@@ -6392,36 +6265,27 @@
     </row>
   </sheetData>
   <mergeCells count="67">
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C56:E56"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="C62:E62"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="C49:E49"/>
-    <mergeCell ref="C54:E54"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="B52:E52"/>
-    <mergeCell ref="C53:E53"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="B77:E77"/>
+    <mergeCell ref="B86:E86"/>
+    <mergeCell ref="B73:E73"/>
+    <mergeCell ref="B74:E74"/>
+    <mergeCell ref="B75:E75"/>
+    <mergeCell ref="B76:E76"/>
+    <mergeCell ref="B80:E80"/>
+    <mergeCell ref="B81:E81"/>
+    <mergeCell ref="B82:E82"/>
+    <mergeCell ref="B78:E78"/>
+    <mergeCell ref="B79:E79"/>
+    <mergeCell ref="B85:E85"/>
+    <mergeCell ref="B83:E83"/>
+    <mergeCell ref="B84:E84"/>
+    <mergeCell ref="B70:E70"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="B71:E71"/>
+    <mergeCell ref="B72:E72"/>
+    <mergeCell ref="B67:E67"/>
+    <mergeCell ref="B68:E68"/>
+    <mergeCell ref="B69:E69"/>
     <mergeCell ref="C31:E31"/>
     <mergeCell ref="C24:E24"/>
     <mergeCell ref="C60:E60"/>
@@ -6438,27 +6302,36 @@
     <mergeCell ref="C39:E39"/>
     <mergeCell ref="C30:E30"/>
     <mergeCell ref="C48:E48"/>
-    <mergeCell ref="B70:E70"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="B71:E71"/>
-    <mergeCell ref="B72:E72"/>
-    <mergeCell ref="B67:E67"/>
-    <mergeCell ref="B68:E68"/>
-    <mergeCell ref="B69:E69"/>
-    <mergeCell ref="B77:E77"/>
-    <mergeCell ref="B86:E86"/>
-    <mergeCell ref="B73:E73"/>
-    <mergeCell ref="B74:E74"/>
-    <mergeCell ref="B75:E75"/>
-    <mergeCell ref="B76:E76"/>
-    <mergeCell ref="B80:E80"/>
-    <mergeCell ref="B81:E81"/>
-    <mergeCell ref="B82:E82"/>
-    <mergeCell ref="B78:E78"/>
-    <mergeCell ref="B79:E79"/>
-    <mergeCell ref="B85:E85"/>
-    <mergeCell ref="B83:E83"/>
-    <mergeCell ref="B84:E84"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C56:E56"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="C54:E54"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="B52:E52"/>
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="C43:E43"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6474,8 +6347,8 @@
   </sheetPr>
   <dimension ref="A3:Y45"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView showGridLines="0" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -6496,91 +6369,91 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:25" ht="18" customHeight="1">
-      <c r="B3" s="205" t="s">
+      <c r="B3" s="216" t="s">
         <v>165</v>
       </c>
-      <c r="C3" s="205"/>
-      <c r="D3" s="205"/>
-      <c r="E3" s="205"/>
-      <c r="F3" s="205"/>
-      <c r="G3" s="205"/>
-      <c r="H3" s="205"/>
-      <c r="I3" s="205"/>
-      <c r="J3" s="205"/>
-      <c r="K3" s="205"/>
-      <c r="L3" s="205"/>
-      <c r="M3" s="205"/>
-      <c r="N3" s="205"/>
+      <c r="C3" s="216"/>
+      <c r="D3" s="216"/>
+      <c r="E3" s="216"/>
+      <c r="F3" s="216"/>
+      <c r="G3" s="216"/>
+      <c r="H3" s="216"/>
+      <c r="I3" s="216"/>
+      <c r="J3" s="216"/>
+      <c r="K3" s="216"/>
+      <c r="L3" s="216"/>
+      <c r="M3" s="216"/>
+      <c r="N3" s="216"/>
     </row>
     <row r="4" spans="2:25" ht="11.25" customHeight="1">
       <c r="B4" s="4"/>
     </row>
     <row r="5" spans="2:25" ht="15" customHeight="1"/>
     <row r="6" spans="2:25" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="B6" s="207" t="s">
+      <c r="B6" s="211" t="s">
         <v>173</v>
       </c>
-      <c r="C6" s="208"/>
-      <c r="D6" s="202" t="s">
-        <v>172</v>
-      </c>
-      <c r="E6" s="203"/>
-      <c r="F6" s="204"/>
-      <c r="G6" s="206"/>
-      <c r="H6" s="206"/>
+      <c r="C6" s="212"/>
+      <c r="D6" s="213" t="s">
+        <v>244</v>
+      </c>
+      <c r="E6" s="214"/>
+      <c r="F6" s="215"/>
+      <c r="G6" s="217"/>
+      <c r="H6" s="217"/>
       <c r="Y6" s="3"/>
     </row>
     <row r="7" spans="2:25" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="B7" s="207" t="s">
-        <v>115</v>
-      </c>
-      <c r="C7" s="208"/>
-      <c r="D7" s="202" t="s">
-        <v>171</v>
-      </c>
-      <c r="E7" s="203"/>
-      <c r="F7" s="204"/>
+      <c r="B7" s="211" t="s">
+        <v>245</v>
+      </c>
+      <c r="C7" s="212"/>
+      <c r="D7" s="213" t="s">
+        <v>242</v>
+      </c>
+      <c r="E7" s="214"/>
+      <c r="F7" s="215"/>
       <c r="Y7" s="3"/>
     </row>
     <row r="8" spans="2:25" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="B8" s="207" t="s">
+      <c r="B8" s="211" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="208"/>
-      <c r="D8" s="202" t="s">
-        <v>176</v>
-      </c>
-      <c r="E8" s="203"/>
-      <c r="F8" s="204"/>
+      <c r="C8" s="212"/>
+      <c r="D8" s="213" t="s">
+        <v>242</v>
+      </c>
+      <c r="E8" s="214"/>
+      <c r="F8" s="215"/>
       <c r="Y8" s="3"/>
     </row>
     <row r="9" spans="2:25" s="5" customFormat="1" ht="27.75" customHeight="1">
-      <c r="B9" s="207" t="s">
+      <c r="B9" s="211" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="208"/>
+      <c r="C9" s="212"/>
       <c r="D9" s="158">
-        <v>41832</v>
+        <v>42290</v>
       </c>
       <c r="E9" s="108" t="s">
         <v>22</v>
       </c>
       <c r="F9" s="145">
-        <v>41844</v>
+        <v>42290</v>
       </c>
       <c r="H9" s="159"/>
       <c r="Y9" s="3"/>
     </row>
     <row r="10" spans="2:25" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="B10" s="207" t="s">
+      <c r="B10" s="211" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="208"/>
-      <c r="D10" s="202" t="s">
-        <v>195</v>
-      </c>
-      <c r="E10" s="203"/>
-      <c r="F10" s="204"/>
+      <c r="C10" s="212"/>
+      <c r="D10" s="213" t="s">
+        <v>246</v>
+      </c>
+      <c r="E10" s="214"/>
+      <c r="F10" s="215"/>
       <c r="Y10" s="3"/>
     </row>
     <row r="11" spans="2:25" s="20" customFormat="1" ht="15" customHeight="1">
@@ -6642,7 +6515,7 @@
         <v>167</v>
       </c>
       <c r="E13" s="150" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="F13" s="144" t="s">
         <v>172</v>
@@ -6651,10 +6524,10 @@
         <v>171</v>
       </c>
       <c r="H13" s="145">
-        <v>41832</v>
+        <v>42290</v>
       </c>
       <c r="I13" s="145">
-        <v>41832</v>
+        <v>42290</v>
       </c>
       <c r="J13" s="147">
         <v>2</v>
@@ -6681,7 +6554,7 @@
         <v>167</v>
       </c>
       <c r="E14" s="150" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="F14" s="144" t="s">
         <v>172</v>
@@ -6690,10 +6563,10 @@
         <v>171</v>
       </c>
       <c r="H14" s="145">
-        <v>41832</v>
+        <v>42290</v>
       </c>
       <c r="I14" s="145">
-        <v>41832</v>
+        <v>42290</v>
       </c>
       <c r="J14" s="147">
         <v>2</v>
@@ -6720,7 +6593,7 @@
         <v>167</v>
       </c>
       <c r="E15" s="150" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="F15" s="144" t="s">
         <v>172</v>
@@ -6729,10 +6602,10 @@
         <v>171</v>
       </c>
       <c r="H15" s="145">
-        <v>41832</v>
+        <v>42290</v>
       </c>
       <c r="I15" s="145">
-        <v>41832</v>
+        <v>42290</v>
       </c>
       <c r="J15" s="147">
         <v>1.5</v>
@@ -6759,7 +6632,7 @@
         <v>167</v>
       </c>
       <c r="E16" s="150" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F16" s="144" t="s">
         <v>172</v>
@@ -6768,10 +6641,10 @@
         <v>171</v>
       </c>
       <c r="H16" s="145">
-        <v>41832</v>
+        <v>42290</v>
       </c>
       <c r="I16" s="145">
-        <v>41832</v>
+        <v>42290</v>
       </c>
       <c r="J16" s="147">
         <v>2</v>
@@ -6798,7 +6671,7 @@
         <v>167</v>
       </c>
       <c r="E17" s="150" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="F17" s="144" t="s">
         <v>172</v>
@@ -6807,10 +6680,10 @@
         <v>171</v>
       </c>
       <c r="H17" s="145">
-        <v>41832</v>
+        <v>42290</v>
       </c>
       <c r="I17" s="145">
-        <v>41832</v>
+        <v>42290</v>
       </c>
       <c r="J17" s="147">
         <v>2</v>
@@ -6837,7 +6710,7 @@
         <v>167</v>
       </c>
       <c r="E18" s="150" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="F18" s="144" t="s">
         <v>172</v>
@@ -6846,10 +6719,10 @@
         <v>171</v>
       </c>
       <c r="H18" s="145">
-        <v>41832</v>
+        <v>42290</v>
       </c>
       <c r="I18" s="145">
-        <v>41832</v>
+        <v>42290</v>
       </c>
       <c r="J18" s="147">
         <v>3</v>
@@ -6876,7 +6749,7 @@
         <v>167</v>
       </c>
       <c r="E19" s="150" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="F19" s="144" t="s">
         <v>172</v>
@@ -6885,10 +6758,10 @@
         <v>171</v>
       </c>
       <c r="H19" s="145">
-        <v>41832</v>
+        <v>42290</v>
       </c>
       <c r="I19" s="145">
-        <v>41832</v>
+        <v>42290</v>
       </c>
       <c r="J19" s="147">
         <v>3</v>
@@ -6915,7 +6788,7 @@
         <v>168</v>
       </c>
       <c r="E20" s="151" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="F20" s="144" t="s">
         <v>172</v>
@@ -6924,10 +6797,10 @@
         <v>171</v>
       </c>
       <c r="H20" s="145">
-        <v>41832</v>
+        <v>42290</v>
       </c>
       <c r="I20" s="145">
-        <v>41832</v>
+        <v>42290</v>
       </c>
       <c r="J20" s="147">
         <v>1</v>
@@ -6954,7 +6827,7 @@
         <v>168</v>
       </c>
       <c r="E21" s="153" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="F21" s="144" t="s">
         <v>172</v>
@@ -6963,10 +6836,10 @@
         <v>171</v>
       </c>
       <c r="H21" s="145">
-        <v>41832</v>
+        <v>42290</v>
       </c>
       <c r="I21" s="145">
-        <v>41832</v>
+        <v>42290</v>
       </c>
       <c r="J21" s="147">
         <v>1</v>
@@ -6993,7 +6866,7 @@
         <v>168</v>
       </c>
       <c r="E22" s="153" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="F22" s="144" t="s">
         <v>172</v>
@@ -7002,10 +6875,10 @@
         <v>171</v>
       </c>
       <c r="H22" s="145">
-        <v>41832</v>
+        <v>42290</v>
       </c>
       <c r="I22" s="145">
-        <v>41832</v>
+        <v>42290</v>
       </c>
       <c r="J22" s="147">
         <v>1</v>
@@ -7032,7 +6905,7 @@
         <v>168</v>
       </c>
       <c r="E23" s="153" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="F23" s="144" t="s">
         <v>172</v>
@@ -7041,10 +6914,10 @@
         <v>171</v>
       </c>
       <c r="H23" s="145">
-        <v>41832</v>
+        <v>42290</v>
       </c>
       <c r="I23" s="145">
-        <v>41832</v>
+        <v>42290</v>
       </c>
       <c r="J23" s="147">
         <v>1.5</v>
@@ -7071,7 +6944,7 @@
         <v>168</v>
       </c>
       <c r="E24" s="153" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="F24" s="144" t="s">
         <v>172</v>
@@ -7080,10 +6953,10 @@
         <v>171</v>
       </c>
       <c r="H24" s="145">
-        <v>41832</v>
+        <v>42290</v>
       </c>
       <c r="I24" s="145">
-        <v>41832</v>
+        <v>42290</v>
       </c>
       <c r="J24" s="147">
         <v>1</v>
@@ -7110,7 +6983,7 @@
         <v>168</v>
       </c>
       <c r="E25" s="154" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="F25" s="144" t="s">
         <v>172</v>
@@ -7119,10 +6992,10 @@
         <v>171</v>
       </c>
       <c r="H25" s="145">
-        <v>41832</v>
+        <v>42290</v>
       </c>
       <c r="I25" s="145">
-        <v>41832</v>
+        <v>42290</v>
       </c>
       <c r="J25" s="147">
         <v>2</v>
@@ -7149,7 +7022,7 @@
         <v>166</v>
       </c>
       <c r="E26" s="156" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="F26" s="144" t="s">
         <v>172</v>
@@ -7158,10 +7031,10 @@
         <v>171</v>
       </c>
       <c r="H26" s="145">
-        <v>41832</v>
+        <v>42290</v>
       </c>
       <c r="I26" s="145">
-        <v>41832</v>
+        <v>42290</v>
       </c>
       <c r="J26" s="147">
         <v>1</v>
@@ -7188,7 +7061,7 @@
         <v>166</v>
       </c>
       <c r="E27" s="157" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F27" s="144" t="s">
         <v>172</v>
@@ -7197,10 +7070,10 @@
         <v>171</v>
       </c>
       <c r="H27" s="145">
-        <v>41832</v>
+        <v>42290</v>
       </c>
       <c r="I27" s="145">
-        <v>41832</v>
+        <v>42290</v>
       </c>
       <c r="J27" s="147">
         <v>2</v>
@@ -7227,7 +7100,7 @@
         <v>166</v>
       </c>
       <c r="E28" s="156" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="F28" s="144" t="s">
         <v>172</v>
@@ -7236,10 +7109,10 @@
         <v>171</v>
       </c>
       <c r="H28" s="145">
-        <v>41832</v>
+        <v>42290</v>
       </c>
       <c r="I28" s="145">
-        <v>41832</v>
+        <v>42290</v>
       </c>
       <c r="J28" s="147">
         <v>2.5</v>
@@ -7267,7 +7140,7 @@
         <v>166</v>
       </c>
       <c r="E29" s="151" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F29" s="144" t="s">
         <v>172</v>
@@ -7276,10 +7149,10 @@
         <v>171</v>
       </c>
       <c r="H29" s="145">
-        <v>41832</v>
+        <v>42290</v>
       </c>
       <c r="I29" s="145">
-        <v>41832</v>
+        <v>42290</v>
       </c>
       <c r="J29" s="147">
         <v>2</v>
@@ -7307,7 +7180,7 @@
         <v>166</v>
       </c>
       <c r="E30" s="151" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F30" s="144" t="s">
         <v>172</v>
@@ -7316,10 +7189,10 @@
         <v>171</v>
       </c>
       <c r="H30" s="145">
-        <v>41832</v>
+        <v>42290</v>
       </c>
       <c r="I30" s="145">
-        <v>41832</v>
+        <v>42290</v>
       </c>
       <c r="J30" s="147">
         <v>1.5</v>
@@ -7344,10 +7217,10 @@
         <v>156</v>
       </c>
       <c r="D31" s="160" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="E31" s="153" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="F31" s="144" t="s">
         <v>172</v>
@@ -7356,10 +7229,10 @@
         <v>171</v>
       </c>
       <c r="H31" s="145">
-        <v>41832</v>
+        <v>42290</v>
       </c>
       <c r="I31" s="145">
-        <v>41832</v>
+        <v>42290</v>
       </c>
       <c r="J31" s="147">
         <v>1.5</v>
@@ -7384,10 +7257,10 @@
         <v>156</v>
       </c>
       <c r="D32" s="160" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="E32" s="153" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="F32" s="144" t="s">
         <v>172</v>
@@ -7396,10 +7269,10 @@
         <v>171</v>
       </c>
       <c r="H32" s="145">
-        <v>41832</v>
+        <v>42290</v>
       </c>
       <c r="I32" s="145">
-        <v>41832</v>
+        <v>42290</v>
       </c>
       <c r="J32" s="147">
         <v>1</v>
@@ -7424,10 +7297,10 @@
         <v>156</v>
       </c>
       <c r="D33" s="160" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="E33" s="153" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="F33" s="144" t="s">
         <v>172</v>
@@ -7436,10 +7309,10 @@
         <v>171</v>
       </c>
       <c r="H33" s="145">
-        <v>41832</v>
+        <v>42290</v>
       </c>
       <c r="I33" s="145">
-        <v>41832</v>
+        <v>42290</v>
       </c>
       <c r="J33" s="147">
         <v>0.5</v>
@@ -7467,7 +7340,7 @@
         <v>170</v>
       </c>
       <c r="E34" s="164" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F34" s="165" t="s">
         <v>172</v>
@@ -7475,19 +7348,19 @@
       <c r="G34" s="165" t="s">
         <v>171</v>
       </c>
-      <c r="H34" s="166">
-        <v>41832</v>
-      </c>
-      <c r="I34" s="166">
-        <v>41832</v>
-      </c>
-      <c r="J34" s="167">
+      <c r="H34" s="145">
+        <v>42290</v>
+      </c>
+      <c r="I34" s="145">
+        <v>42290</v>
+      </c>
+      <c r="J34" s="166">
         <v>1.5</v>
       </c>
-      <c r="K34" s="168">
+      <c r="K34" s="167">
         <v>41979</v>
       </c>
-      <c r="L34" s="169">
+      <c r="L34" s="168">
         <v>41840</v>
       </c>
       <c r="M34" s="105">
@@ -7504,10 +7377,10 @@
         <v>156</v>
       </c>
       <c r="D35" s="160" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="E35" s="144" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="F35" s="144" t="s">
         <v>172</v>
@@ -7516,10 +7389,10 @@
         <v>171</v>
       </c>
       <c r="H35" s="145">
-        <v>41832</v>
+        <v>42290</v>
       </c>
       <c r="I35" s="145">
-        <v>41832</v>
+        <v>42290</v>
       </c>
       <c r="J35" s="147">
         <v>1.5</v>
@@ -7545,7 +7418,7 @@
         <v>170</v>
       </c>
       <c r="E36" s="144" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="F36" s="144" t="s">
         <v>172</v>
@@ -7554,10 +7427,10 @@
         <v>171</v>
       </c>
       <c r="H36" s="145">
-        <v>41832</v>
+        <v>42290</v>
       </c>
       <c r="I36" s="145">
-        <v>41832</v>
+        <v>42290</v>
       </c>
       <c r="J36" s="147">
         <v>2</v>
@@ -7665,17 +7538,17 @@
     <row r="45" spans="1:14" ht="12.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D10:F10"/>
     <mergeCell ref="D7:F7"/>
     <mergeCell ref="B3:N3"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="D6:F6"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D10:F10"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="4">
@@ -7697,8 +7570,7 @@
   <headerFooter alignWithMargins="0">
     <oddFooter xml:space="preserve">&amp;LRev. 1.0&amp;CFecha Efectiva: 16/06/2008&amp;RPágina &amp;P de &amp;N </oddFooter>
   </headerFooter>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -7708,10 +7580,10 @@
   <dimension ref="A1:O50"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="4" topLeftCell="F11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="4" topLeftCell="F5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="G14" sqref="G14"/>
+      <selection pane="bottomRight" activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="11.25"/>
@@ -7732,22 +7604,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="29" customFormat="1" ht="64.5" customHeight="1" thickBot="1">
-      <c r="A1" s="209" t="s">
+      <c r="A1" s="218" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="210"/>
-      <c r="C1" s="210"/>
-      <c r="D1" s="210"/>
-      <c r="E1" s="210"/>
-      <c r="F1" s="210"/>
-      <c r="G1" s="210"/>
-      <c r="H1" s="210"/>
-      <c r="I1" s="210"/>
-      <c r="J1" s="210"/>
-      <c r="K1" s="210"/>
-      <c r="L1" s="210"/>
-      <c r="M1" s="210"/>
-      <c r="N1" s="211"/>
+      <c r="B1" s="219"/>
+      <c r="C1" s="219"/>
+      <c r="D1" s="219"/>
+      <c r="E1" s="219"/>
+      <c r="F1" s="219"/>
+      <c r="G1" s="219"/>
+      <c r="H1" s="219"/>
+      <c r="I1" s="219"/>
+      <c r="J1" s="219"/>
+      <c r="K1" s="219"/>
+      <c r="L1" s="219"/>
+      <c r="M1" s="219"/>
+      <c r="N1" s="220"/>
     </row>
     <row r="2" spans="1:15" s="29" customFormat="1" ht="11.45" customHeight="1">
       <c r="A2" s="30"/>
@@ -7829,7 +7701,7 @@
         <v>Desarrollo de Sistemas</v>
       </c>
       <c r="D5" s="112" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="E5" s="111" t="str">
         <f>VLOOKUP(B5,Planificación!$B$13:$F$87,5,FALSE)</f>
@@ -7840,7 +7712,7 @@
         <v>BC</v>
       </c>
       <c r="G5" s="114" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="H5" s="113" t="s">
         <v>153</v>
@@ -7875,7 +7747,7 @@
         <v>Desarrollo de Sistemas</v>
       </c>
       <c r="D6" s="112" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E6" s="111" t="str">
         <f>VLOOKUP(B6,Planificación!$B$13:$F$87,5,FALSE)</f>
@@ -7886,7 +7758,7 @@
         <v>BC</v>
       </c>
       <c r="G6" s="114" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="H6" s="113" t="s">
         <v>153</v>
@@ -7921,7 +7793,7 @@
         <v>Desarrollo de Sistemas</v>
       </c>
       <c r="D7" s="112" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E7" s="111" t="str">
         <f>VLOOKUP(B7,Planificación!$B$13:$F$87,5,FALSE)</f>
@@ -7932,7 +7804,7 @@
         <v>BC</v>
       </c>
       <c r="G7" s="114" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="H7" s="113" t="s">
         <v>153</v>
@@ -7959,93 +7831,93 @@
       <c r="A8" s="109">
         <v>4</v>
       </c>
-      <c r="B8" s="233">
+      <c r="B8" s="169">
         <v>3</v>
       </c>
-      <c r="C8" s="234" t="str">
+      <c r="C8" s="170" t="str">
         <f>VLOOKUP(B8,Planificación!$B$13:$E$87,2,FALSE)</f>
         <v>Desarrollo de Sistemas</v>
       </c>
-      <c r="D8" s="235" t="s">
-        <v>216</v>
-      </c>
-      <c r="E8" s="234" t="str">
+      <c r="D8" s="171" t="s">
+        <v>211</v>
+      </c>
+      <c r="E8" s="170" t="str">
         <f>VLOOKUP(B8,Planificación!$B$13:$F$87,5,FALSE)</f>
         <v>YM</v>
       </c>
-      <c r="F8" s="234" t="str">
+      <c r="F8" s="170" t="str">
         <f>VLOOKUP(B8,Planificación!$B$13:$G$87,6,FALSE)</f>
         <v>BC</v>
       </c>
-      <c r="G8" s="236" t="s">
-        <v>244</v>
-      </c>
-      <c r="H8" s="237" t="s">
+      <c r="G8" s="172" t="s">
+        <v>239</v>
+      </c>
+      <c r="H8" s="173" t="s">
         <v>153</v>
       </c>
-      <c r="I8" s="237" t="s">
+      <c r="I8" s="173" t="s">
         <v>95</v>
       </c>
-      <c r="J8" s="237" t="s">
+      <c r="J8" s="173" t="s">
         <v>172</v>
       </c>
-      <c r="K8" s="238"/>
-      <c r="L8" s="239">
+      <c r="K8" s="174"/>
+      <c r="L8" s="175">
         <v>41835</v>
       </c>
-      <c r="M8" s="239">
+      <c r="M8" s="175">
         <v>41841</v>
       </c>
-      <c r="N8" s="240">
+      <c r="N8" s="176">
         <v>1</v>
       </c>
-      <c r="O8" s="241"/>
+      <c r="O8" s="177"/>
     </row>
     <row r="9" spans="1:15" ht="24">
       <c r="A9" s="109">
         <v>5</v>
       </c>
-      <c r="B9" s="233">
+      <c r="B9" s="169">
         <v>3</v>
       </c>
-      <c r="C9" s="234" t="str">
+      <c r="C9" s="170" t="str">
         <f>VLOOKUP(B9,Planificación!$B$13:$E$87,2,FALSE)</f>
         <v>Desarrollo de Sistemas</v>
       </c>
-      <c r="D9" s="235" t="s">
-        <v>217</v>
-      </c>
-      <c r="E9" s="234" t="str">
+      <c r="D9" s="171" t="s">
+        <v>212</v>
+      </c>
+      <c r="E9" s="170" t="str">
         <f>VLOOKUP(B9,Planificación!$B$13:$F$87,5,FALSE)</f>
         <v>YM</v>
       </c>
-      <c r="F9" s="234" t="str">
+      <c r="F9" s="170" t="str">
         <f>VLOOKUP(B9,Planificación!$B$13:$G$87,6,FALSE)</f>
         <v>BC</v>
       </c>
-      <c r="G9" s="236" t="s">
-        <v>218</v>
-      </c>
-      <c r="H9" s="237" t="s">
+      <c r="G9" s="172" t="s">
+        <v>213</v>
+      </c>
+      <c r="H9" s="173" t="s">
         <v>153</v>
       </c>
-      <c r="I9" s="237" t="s">
+      <c r="I9" s="173" t="s">
         <v>95</v>
       </c>
-      <c r="J9" s="237" t="s">
-        <v>219</v>
-      </c>
-      <c r="K9" s="238"/>
-      <c r="L9" s="239">
+      <c r="J9" s="173" t="s">
+        <v>214</v>
+      </c>
+      <c r="K9" s="174"/>
+      <c r="L9" s="175">
         <v>41835</v>
       </c>
-      <c r="M9" s="239">
+      <c r="M9" s="175">
         <v>41841</v>
       </c>
-      <c r="N9" s="240">
+      <c r="N9" s="176">
         <v>1</v>
       </c>
-      <c r="O9" s="241"/>
+      <c r="O9" s="177"/>
     </row>
     <row r="10" spans="1:15" ht="24">
       <c r="A10" s="109">
@@ -8059,7 +7931,7 @@
         <v>Desarrollo de Sistemas</v>
       </c>
       <c r="D10" s="112" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="E10" s="111" t="str">
         <f>VLOOKUP(B10,Planificación!$B$13:$F$87,5,FALSE)</f>
@@ -8070,7 +7942,7 @@
         <v>BC</v>
       </c>
       <c r="G10" s="114" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="H10" s="113" t="s">
         <v>153</v>
@@ -8104,7 +7976,7 @@
         <v>156</v>
       </c>
       <c r="D11" s="112" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="E11" s="111" t="s">
         <v>172</v>
@@ -8113,7 +7985,7 @@
         <v>171</v>
       </c>
       <c r="G11" s="161" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H11" s="113" t="s">
         <v>153</v>
@@ -8147,7 +8019,7 @@
         <v>156</v>
       </c>
       <c r="D12" s="112" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="E12" s="111" t="s">
         <v>172</v>
@@ -8156,7 +8028,7 @@
         <v>171</v>
       </c>
       <c r="G12" s="114" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="H12" s="113" t="s">
         <v>153</v>
@@ -8191,7 +8063,7 @@
         <v>Desarrollo de Sistemas</v>
       </c>
       <c r="D13" s="112" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E13" s="111" t="str">
         <f>VLOOKUP(B13,Planificación!$B$13:$F$87,5,FALSE)</f>
@@ -8202,7 +8074,7 @@
         <v>BC</v>
       </c>
       <c r="G13" s="114" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="H13" s="113" t="s">
         <v>153</v>
@@ -8225,51 +8097,51 @@
       </c>
       <c r="O13" s="130"/>
     </row>
-    <row r="14" spans="1:15" s="242" customFormat="1" ht="24">
+    <row r="14" spans="1:15" s="178" customFormat="1" ht="24">
       <c r="A14" s="109">
         <v>10</v>
       </c>
-      <c r="B14" s="233">
+      <c r="B14" s="169">
         <v>3</v>
       </c>
-      <c r="C14" s="234" t="str">
+      <c r="C14" s="170" t="str">
         <f>VLOOKUP(B14,Planificación!$B$13:$E$87,2,FALSE)</f>
         <v>Desarrollo de Sistemas</v>
       </c>
-      <c r="D14" s="235" t="s">
-        <v>225</v>
-      </c>
-      <c r="E14" s="234" t="str">
+      <c r="D14" s="171" t="s">
+        <v>220</v>
+      </c>
+      <c r="E14" s="170" t="str">
         <f>VLOOKUP(B14,Planificación!$B$13:$F$87,5,FALSE)</f>
         <v>YM</v>
       </c>
-      <c r="F14" s="234" t="str">
+      <c r="F14" s="170" t="str">
         <f>VLOOKUP(B14,Planificación!$B$13:$G$87,6,FALSE)</f>
         <v>BC</v>
       </c>
-      <c r="G14" s="243" t="s">
-        <v>228</v>
-      </c>
-      <c r="H14" s="237" t="s">
+      <c r="G14" s="179" t="s">
+        <v>223</v>
+      </c>
+      <c r="H14" s="173" t="s">
         <v>153</v>
       </c>
-      <c r="I14" s="237" t="s">
+      <c r="I14" s="173" t="s">
         <v>95</v>
       </c>
-      <c r="J14" s="237" t="s">
+      <c r="J14" s="173" t="s">
         <v>172</v>
       </c>
-      <c r="K14" s="238"/>
-      <c r="L14" s="239">
+      <c r="K14" s="174"/>
+      <c r="L14" s="175">
         <v>41835</v>
       </c>
-      <c r="M14" s="239">
+      <c r="M14" s="175">
         <v>41841</v>
       </c>
-      <c r="N14" s="240">
+      <c r="N14" s="176">
         <v>1</v>
       </c>
-      <c r="O14" s="241"/>
+      <c r="O14" s="177"/>
     </row>
     <row r="15" spans="1:15" ht="24">
       <c r="A15" s="109">
@@ -8283,7 +8155,7 @@
         <v>Desarrollo de Sistemas</v>
       </c>
       <c r="D15" s="112" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="E15" s="111" t="str">
         <f>VLOOKUP(B15,Planificación!$B$13:$F$87,5,FALSE)</f>
@@ -8294,7 +8166,7 @@
         <v>BC</v>
       </c>
       <c r="G15" s="114" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="H15" s="113" t="s">
         <v>154</v>
@@ -8303,7 +8175,7 @@
         <v>95</v>
       </c>
       <c r="J15" s="113" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K15" s="115"/>
       <c r="L15" s="116">
@@ -8329,7 +8201,7 @@
         <v>Desarrollo de Sistemas</v>
       </c>
       <c r="D16" s="112" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="E16" s="111" t="str">
         <f>VLOOKUP(B16,Planificación!$B$13:$F$87,5,FALSE)</f>
@@ -8340,7 +8212,7 @@
         <v>BC</v>
       </c>
       <c r="G16" s="114" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H16" s="113" t="s">
         <v>153</v>
@@ -8349,7 +8221,7 @@
         <v>95</v>
       </c>
       <c r="J16" s="113" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="K16" s="115"/>
       <c r="L16" s="116">
@@ -8375,7 +8247,7 @@
         <v>Desarrollo de Sistemas</v>
       </c>
       <c r="D17" s="112" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="E17" s="111" t="str">
         <f>VLOOKUP(B17,Planificación!$B$13:$F$87,5,FALSE)</f>
@@ -8386,7 +8258,7 @@
         <v>BC</v>
       </c>
       <c r="G17" s="114" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="H17" s="113" t="s">
         <v>153</v>
@@ -8395,7 +8267,7 @@
         <v>95</v>
       </c>
       <c r="J17" s="113" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="K17" s="115"/>
       <c r="L17" s="116">
@@ -8421,7 +8293,7 @@
         <v>Desarrollo de Sistemas</v>
       </c>
       <c r="D18" s="112" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E18" s="111" t="str">
         <f>VLOOKUP(B18,Planificación!$B$13:$F$87,5,FALSE)</f>
@@ -8432,7 +8304,7 @@
         <v>BC</v>
       </c>
       <c r="G18" s="114" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="H18" s="113" t="s">
         <v>153</v>
@@ -8467,7 +8339,7 @@
         <v>Desarrollo de Sistemas</v>
       </c>
       <c r="D19" s="112" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="E19" s="111" t="str">
         <f>VLOOKUP(B19,Planificación!$B$13:$F$87,5,FALSE)</f>
@@ -8478,7 +8350,7 @@
         <v>BC</v>
       </c>
       <c r="G19" s="114" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="H19" s="113" t="s">
         <v>153</v>
@@ -8513,7 +8385,7 @@
         <v>Desarrollo de Sistemas</v>
       </c>
       <c r="D20" s="112" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="E20" s="111" t="str">
         <f>VLOOKUP(B20,Planificación!$B$13:$F$87,5,FALSE)</f>
@@ -8524,7 +8396,7 @@
         <v>BC</v>
       </c>
       <c r="G20" s="114" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="H20" s="113" t="s">
         <v>153</v>
@@ -8559,7 +8431,7 @@
         <v>Desarrollo de Sistemas</v>
       </c>
       <c r="D21" s="112" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="E21" s="111" t="str">
         <f>VLOOKUP(B21,Planificación!$B$13:$F$87,5,FALSE)</f>
@@ -8570,7 +8442,7 @@
         <v>BC</v>
       </c>
       <c r="G21" s="114" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="H21" s="113" t="s">
         <v>153</v>
@@ -8605,7 +8477,7 @@
         <v>Desarrollo de Sistemas</v>
       </c>
       <c r="D22" s="112" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="E22" s="111" t="str">
         <f>VLOOKUP(B22,Planificación!$B$13:$F$87,5,FALSE)</f>
@@ -8616,7 +8488,7 @@
         <v>BC</v>
       </c>
       <c r="G22" s="114" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="H22" s="113" t="s">
         <v>153</v>
@@ -8651,7 +8523,7 @@
         <v>Desarrollo de Sistemas</v>
       </c>
       <c r="D23" s="112" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="E23" s="111" t="str">
         <f>VLOOKUP(B23,Planificación!$B$13:$F$87,5,FALSE)</f>
@@ -8662,7 +8534,7 @@
         <v>BC</v>
       </c>
       <c r="G23" s="114" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="H23" s="113" t="s">
         <v>153</v>
@@ -8697,7 +8569,7 @@
         <v>Desarrollo de Sistemas</v>
       </c>
       <c r="D24" s="112" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="E24" s="111" t="str">
         <f>VLOOKUP(B24,Planificación!$B$13:$F$87,5,FALSE)</f>
@@ -8708,7 +8580,7 @@
         <v>BC</v>
       </c>
       <c r="G24" s="114" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="H24" s="113" t="s">
         <v>153</v>
@@ -8743,7 +8615,7 @@
         <v>Desarrollo de Sistemas</v>
       </c>
       <c r="D25" s="112" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="E25" s="111" t="str">
         <f>VLOOKUP(B25,Planificación!$B$13:$F$87,5,FALSE)</f>
@@ -8754,7 +8626,7 @@
         <v>BC</v>
       </c>
       <c r="G25" s="114" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="H25" s="113" t="s">
         <v>153</v>
@@ -8789,7 +8661,7 @@
         <v>Desarrollo de Sistemas</v>
       </c>
       <c r="D26" s="112" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="E26" s="111" t="str">
         <f>VLOOKUP(B26,Planificación!$B$13:$F$87,5,FALSE)</f>
@@ -8800,7 +8672,7 @@
         <v>BC</v>
       </c>
       <c r="G26" s="114" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="H26" s="113" t="s">
         <v>153</v>
@@ -8835,7 +8707,7 @@
         <v>Desarrollo de Sistemas</v>
       </c>
       <c r="D27" s="112" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="E27" s="111" t="str">
         <f>VLOOKUP(B27,Planificación!$B$13:$F$87,5,FALSE)</f>
@@ -8846,7 +8718,7 @@
         <v>BC</v>
       </c>
       <c r="G27" s="114" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="H27" s="113" t="s">
         <v>153</v>
@@ -8881,7 +8753,7 @@
         <v>Desarrollo de Sistemas</v>
       </c>
       <c r="D28" s="112" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="E28" s="111" t="str">
         <f>VLOOKUP(B28,Planificación!$B$13:$F$87,5,FALSE)</f>
@@ -8892,7 +8764,7 @@
         <v>BC</v>
       </c>
       <c r="G28" s="114" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="H28" s="113" t="s">
         <v>153</v>
@@ -9142,7 +9014,7 @@
   <sheetPr codeName="Hoja5"/>
   <dimension ref="A2:K62"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A19" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
@@ -9158,107 +9030,107 @@
   <sheetData>
     <row r="2" spans="1:11" s="1" customFormat="1" ht="17.25" customHeight="1">
       <c r="A2" s="13"/>
-      <c r="C2" s="212" t="s">
+      <c r="C2" s="234" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="212"/>
-      <c r="E2" s="212"/>
-      <c r="F2" s="212"/>
-      <c r="G2" s="212"/>
-      <c r="H2" s="212"/>
-      <c r="I2" s="212"/>
-      <c r="J2" s="212"/>
-      <c r="K2" s="212"/>
+      <c r="D2" s="234"/>
+      <c r="E2" s="234"/>
+      <c r="F2" s="234"/>
+      <c r="G2" s="234"/>
+      <c r="H2" s="234"/>
+      <c r="I2" s="234"/>
+      <c r="J2" s="234"/>
+      <c r="K2" s="234"/>
     </row>
     <row r="3" spans="1:11" s="2" customFormat="1" ht="34.5" customHeight="1">
       <c r="A3" s="14"/>
     </row>
     <row r="4" spans="1:11" s="2" customFormat="1">
       <c r="A4" s="14"/>
-      <c r="C4" s="213" t="s">
+      <c r="C4" s="235" t="s">
         <v>173</v>
       </c>
-      <c r="D4" s="213"/>
-      <c r="E4" s="214" t="str">
+      <c r="D4" s="235"/>
+      <c r="E4" s="224" t="str">
         <f>IF(Planificación!D6&lt;&gt;"",Planificación!D6,"")</f>
-        <v>YM</v>
-      </c>
-      <c r="F4" s="215"/>
-      <c r="G4" s="215"/>
-      <c r="H4" s="215"/>
-      <c r="I4" s="216"/>
+        <v>Roger Apaestegui Ortega</v>
+      </c>
+      <c r="F4" s="225"/>
+      <c r="G4" s="225"/>
+      <c r="H4" s="225"/>
+      <c r="I4" s="226"/>
     </row>
     <row r="5" spans="1:11" s="2" customFormat="1">
       <c r="A5" s="14"/>
-      <c r="C5" s="217" t="str">
+      <c r="C5" s="236" t="str">
         <f>Planificación!B7</f>
-        <v>Gestor de Calidad</v>
-      </c>
-      <c r="D5" s="218"/>
-      <c r="E5" s="214" t="str">
+        <v>Analista de Calidad</v>
+      </c>
+      <c r="D5" s="237"/>
+      <c r="E5" s="224" t="str">
         <f>IF(Planificación!D7&lt;&gt;"",Planificación!D7,"")</f>
-        <v>BC</v>
-      </c>
-      <c r="F5" s="215"/>
-      <c r="G5" s="215"/>
-      <c r="H5" s="215"/>
-      <c r="I5" s="216"/>
+        <v>Julio Leonardo Paredes</v>
+      </c>
+      <c r="F5" s="225"/>
+      <c r="G5" s="225"/>
+      <c r="H5" s="225"/>
+      <c r="I5" s="226"/>
     </row>
     <row r="6" spans="1:11" s="2" customFormat="1">
       <c r="A6" s="14"/>
-      <c r="C6" s="220" t="s">
+      <c r="C6" s="222" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="221"/>
-      <c r="E6" s="214" t="str">
+      <c r="D6" s="223"/>
+      <c r="E6" s="224" t="str">
         <f>IF(Planificación!D8&lt;&gt;"",Planificación!D8,"")</f>
-        <v>HM, JG, RR</v>
-      </c>
-      <c r="F6" s="215"/>
-      <c r="G6" s="215"/>
-      <c r="H6" s="215"/>
-      <c r="I6" s="216"/>
+        <v>Julio Leonardo Paredes</v>
+      </c>
+      <c r="F6" s="225"/>
+      <c r="G6" s="225"/>
+      <c r="H6" s="225"/>
+      <c r="I6" s="226"/>
     </row>
     <row r="7" spans="1:11" s="2" customFormat="1" ht="24" customHeight="1">
       <c r="A7" s="14"/>
-      <c r="C7" s="223" t="s">
+      <c r="C7" s="228" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="223"/>
-      <c r="E7" s="224">
+      <c r="D7" s="228"/>
+      <c r="E7" s="229">
         <f>IF(Planificación!D9&lt;&gt;"",Planificación!D9,"")</f>
-        <v>41832</v>
-      </c>
-      <c r="F7" s="225"/>
-      <c r="G7" s="226" t="s">
+        <v>42290</v>
+      </c>
+      <c r="F7" s="230"/>
+      <c r="G7" s="231" t="s">
         <v>22</v>
       </c>
-      <c r="H7" s="227"/>
+      <c r="H7" s="232"/>
       <c r="I7" s="118">
         <f>IF(Planificación!F9&lt;&gt;"",Planificación!F9,"")</f>
-        <v>41844</v>
+        <v>42290</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="2" customFormat="1">
       <c r="A8" s="14"/>
-      <c r="C8" s="223" t="s">
+      <c r="C8" s="228" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="228"/>
-      <c r="E8" s="214" t="str">
+      <c r="D8" s="233"/>
+      <c r="E8" s="224" t="str">
         <f>IF(Planificación!D10&lt;&gt;"",Planificación!D10,"")</f>
-        <v>JULIO</v>
-      </c>
-      <c r="F8" s="215"/>
-      <c r="G8" s="215"/>
-      <c r="H8" s="215"/>
-      <c r="I8" s="216"/>
+        <v>OCTUBRE</v>
+      </c>
+      <c r="F8" s="225"/>
+      <c r="G8" s="225"/>
+      <c r="H8" s="225"/>
+      <c r="I8" s="226"/>
     </row>
     <row r="13" spans="1:11" ht="15">
-      <c r="C13" s="222" t="s">
+      <c r="C13" s="227" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="222"/>
+      <c r="D13" s="227"/>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
       <c r="G13" s="15"/>
@@ -9342,10 +9214,10 @@
       <c r="E24" s="12"/>
     </row>
     <row r="26" spans="3:5" ht="15" customHeight="1">
-      <c r="C26" s="219" t="s">
+      <c r="C26" s="221" t="s">
         <v>39</v>
       </c>
-      <c r="D26" s="219"/>
+      <c r="D26" s="221"/>
     </row>
     <row r="27" spans="3:5">
       <c r="C27" s="34" t="s">
@@ -9419,10 +9291,10 @@
       </c>
     </row>
     <row r="40" spans="3:4" ht="15">
-      <c r="C40" s="219" t="s">
+      <c r="C40" s="221" t="s">
         <v>108</v>
       </c>
-      <c r="D40" s="219"/>
+      <c r="D40" s="221"/>
     </row>
     <row r="41" spans="3:4">
       <c r="C41" s="123" t="s">
@@ -9452,10 +9324,10 @@
       </c>
     </row>
     <row r="57" spans="3:4" ht="15">
-      <c r="C57" s="219" t="s">
+      <c r="C57" s="221" t="s">
         <v>152</v>
       </c>
-      <c r="D57" s="219"/>
+      <c r="D57" s="221"/>
     </row>
     <row r="58" spans="3:4">
       <c r="C58" s="34" t="s">
@@ -9503,6 +9375,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="C2:K2"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:I4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:I5"/>
     <mergeCell ref="C57:D57"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="E6:I6"/>
@@ -9514,11 +9391,6 @@
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C2:K2"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:I4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:I5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -9592,7 +9464,7 @@
       <c r="H3" s="125" t="s">
         <v>117</v>
       </c>
-      <c r="J3" s="229" t="s">
+      <c r="J3" s="238" t="s">
         <v>117</v>
       </c>
       <c r="K3" s="138" t="s">
@@ -9600,7 +9472,7 @@
       </c>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="230" t="s">
+      <c r="A4" s="239" t="s">
         <v>156</v>
       </c>
       <c r="B4" s="135" t="s">
@@ -9615,13 +9487,13 @@
       <c r="H4" s="125" t="s">
         <v>118</v>
       </c>
-      <c r="J4" s="229"/>
+      <c r="J4" s="238"/>
       <c r="K4" s="138" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="231"/>
+      <c r="A5" s="240"/>
       <c r="B5" s="136" t="s">
         <v>167</v>
       </c>
@@ -9634,13 +9506,13 @@
       <c r="H5" s="125" t="s">
         <v>156</v>
       </c>
-      <c r="J5" s="229"/>
+      <c r="J5" s="238"/>
       <c r="K5" s="138" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="231"/>
+      <c r="A6" s="240"/>
       <c r="B6" s="136" t="s">
         <v>168</v>
       </c>
@@ -9648,13 +9520,13 @@
         <v>155</v>
       </c>
       <c r="H6" s="125"/>
-      <c r="J6" s="229"/>
+      <c r="J6" s="238"/>
       <c r="K6" s="138" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="231"/>
+      <c r="A7" s="240"/>
       <c r="B7" s="136" t="s">
         <v>169</v>
       </c>
@@ -9662,7 +9534,7 @@
         <v>37</v>
       </c>
       <c r="H7" s="125"/>
-      <c r="J7" s="229" t="s">
+      <c r="J7" s="238" t="s">
         <v>126</v>
       </c>
       <c r="K7" s="138" t="s">
@@ -9670,7 +9542,7 @@
       </c>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="231"/>
+      <c r="A8" s="240"/>
       <c r="B8" s="136" t="s">
         <v>170</v>
       </c>
@@ -9678,54 +9550,54 @@
         <v>36</v>
       </c>
       <c r="H8" s="125"/>
-      <c r="J8" s="229"/>
+      <c r="J8" s="238"/>
       <c r="K8" s="138" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="231"/>
+      <c r="A9" s="240"/>
       <c r="B9" s="139"/>
-      <c r="J9" s="229"/>
+      <c r="J9" s="238"/>
       <c r="K9" s="138" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="231"/>
+      <c r="A10" s="240"/>
       <c r="B10" s="136"/>
       <c r="F10" s="131"/>
-      <c r="J10" s="229"/>
+      <c r="J10" s="238"/>
       <c r="K10" s="138" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="231"/>
+      <c r="A11" s="240"/>
       <c r="B11" s="136"/>
       <c r="F11" s="131"/>
-      <c r="J11" s="229"/>
+      <c r="J11" s="238"/>
       <c r="K11" s="138" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="12.75" customHeight="1" thickBot="1">
-      <c r="A12" s="232"/>
+      <c r="A12" s="241"/>
       <c r="B12" s="137"/>
       <c r="F12" s="131"/>
-      <c r="J12" s="229"/>
+      <c r="J12" s="238"/>
       <c r="K12" s="138" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:11">
-      <c r="J13" s="229"/>
+      <c r="J13" s="238"/>
       <c r="K13" s="138" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:11">
-      <c r="J14" s="229" t="s">
+      <c r="J14" s="238" t="s">
         <v>119</v>
       </c>
       <c r="K14" s="138" t="s">
@@ -9733,61 +9605,61 @@
       </c>
     </row>
     <row r="15" spans="1:11">
-      <c r="J15" s="229"/>
+      <c r="J15" s="238"/>
       <c r="K15" s="138" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:11">
-      <c r="J16" s="229"/>
+      <c r="J16" s="238"/>
       <c r="K16" s="138" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="17" spans="10:11">
-      <c r="J17" s="229"/>
+      <c r="J17" s="238"/>
       <c r="K17" s="138" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="18" spans="10:11">
-      <c r="J18" s="229"/>
+      <c r="J18" s="238"/>
       <c r="K18" s="138" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="19" spans="10:11">
-      <c r="J19" s="229"/>
+      <c r="J19" s="238"/>
       <c r="K19" s="138" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="20" spans="10:11">
-      <c r="J20" s="229"/>
+      <c r="J20" s="238"/>
       <c r="K20" s="138" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="21" spans="10:11">
-      <c r="J21" s="229"/>
+      <c r="J21" s="238"/>
       <c r="K21" s="138" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="22" spans="10:11">
-      <c r="J22" s="229"/>
+      <c r="J22" s="238"/>
       <c r="K22" s="138" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="23" spans="10:11">
-      <c r="J23" s="229"/>
+      <c r="J23" s="238"/>
       <c r="K23" s="138" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="24" spans="10:11">
-      <c r="J24" s="229" t="s">
+      <c r="J24" s="238" t="s">
         <v>120</v>
       </c>
       <c r="K24" s="138" t="s">
@@ -9795,43 +9667,43 @@
       </c>
     </row>
     <row r="25" spans="10:11">
-      <c r="J25" s="229"/>
+      <c r="J25" s="238"/>
       <c r="K25" s="138" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="26" spans="10:11">
-      <c r="J26" s="229"/>
+      <c r="J26" s="238"/>
       <c r="K26" s="138" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="27" spans="10:11">
-      <c r="J27" s="229"/>
+      <c r="J27" s="238"/>
       <c r="K27" s="138" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="28" spans="10:11">
-      <c r="J28" s="229"/>
+      <c r="J28" s="238"/>
       <c r="K28" s="138" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="29" spans="10:11">
-      <c r="J29" s="229"/>
+      <c r="J29" s="238"/>
       <c r="K29" s="138" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="30" spans="10:11">
-      <c r="J30" s="229"/>
+      <c r="J30" s="238"/>
       <c r="K30" s="138" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="31" spans="10:11">
-      <c r="J31" s="229" t="s">
+      <c r="J31" s="238" t="s">
         <v>121</v>
       </c>
       <c r="K31" s="138" t="s">
@@ -9839,31 +9711,31 @@
       </c>
     </row>
     <row r="32" spans="10:11">
-      <c r="J32" s="229"/>
+      <c r="J32" s="238"/>
       <c r="K32" s="138" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="33" spans="10:11">
-      <c r="J33" s="229"/>
+      <c r="J33" s="238"/>
       <c r="K33" s="138" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="34" spans="10:11">
-      <c r="J34" s="229"/>
+      <c r="J34" s="238"/>
       <c r="K34" s="138" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="35" spans="10:11">
-      <c r="J35" s="229"/>
+      <c r="J35" s="238"/>
       <c r="K35" s="138" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="36" spans="10:11">
-      <c r="J36" s="229" t="s">
+      <c r="J36" s="238" t="s">
         <v>122</v>
       </c>
       <c r="K36" s="138" t="s">
@@ -9871,37 +9743,37 @@
       </c>
     </row>
     <row r="37" spans="10:11">
-      <c r="J37" s="229"/>
+      <c r="J37" s="238"/>
       <c r="K37" s="138" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="38" spans="10:11">
-      <c r="J38" s="229"/>
+      <c r="J38" s="238"/>
       <c r="K38" s="138" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="39" spans="10:11">
-      <c r="J39" s="229"/>
+      <c r="J39" s="238"/>
       <c r="K39" s="138" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="40" spans="10:11">
-      <c r="J40" s="229"/>
+      <c r="J40" s="238"/>
       <c r="K40" s="138" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="41" spans="10:11">
-      <c r="J41" s="229"/>
+      <c r="J41" s="238"/>
       <c r="K41" s="138" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="42" spans="10:11">
-      <c r="J42" s="229"/>
+      <c r="J42" s="238"/>
       <c r="K42" s="138" t="s">
         <v>131</v>
       </c>

</xml_diff>